<commit_message>
Updated SRS and Database Script
-I refined the SRS Document.
-I updated the burn-down chart to reflect changes in the document.
-I added flags to the database.
</commit_message>
<xml_diff>
--- a/Burn Down Chart.xlsx
+++ b/Burn Down Chart.xlsx
@@ -154,62 +154,86 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$19</c:f>
+              <c:f>Sheet1!$A$2:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>mmmm\ d</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>42062</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>42063</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42064</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>42065</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>42066</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>42067</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>42068</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>42069</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>42070</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42071</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>42072</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>42073</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>42074</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>42075</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>42076</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="15">
+                  <c:v>42077</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42078</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>42079</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="18">
                   <c:v>42080</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="19">
                   <c:v>42081</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="20">
                   <c:v>42082</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="21">
                   <c:v>42083</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22">
+                  <c:v>42084</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>42085</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>42086</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="25">
                   <c:v>42087</c:v>
                 </c:pt>
               </c:numCache>
@@ -217,62 +241,86 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$19</c:f>
+              <c:f>Sheet1!$B$2:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>270.00000000000011</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>259.2000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>248.40000000000012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>237.60000000000011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>226.8000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>216.00000000000009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>205.20000000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>194.40000000000006</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>183.60000000000005</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="9">
                   <c:v>172.80000000000004</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="10">
                   <c:v>162.00000000000003</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
                   <c:v>151.20000000000002</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="12">
                   <c:v>140.4</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="13">
                   <c:v>129.6</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="14">
                   <c:v>118.79999999999998</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="15">
                   <c:v>107.99999999999999</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="16">
                   <c:v>97.199999999999989</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="17">
                   <c:v>86.399999999999991</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="18">
                   <c:v>75.599999999999994</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="19">
                   <c:v>64.8</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="20">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="21">
                   <c:v>43.2</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="22">
                   <c:v>32.400000000000006</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="23">
                   <c:v>21.6</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="24">
                   <c:v>10.8</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="25">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -299,62 +347,86 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$19</c:f>
+              <c:f>Sheet1!$A$2:$A$27</c:f>
               <c:numCache>
                 <c:formatCode>mmmm\ d</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>42062</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>42063</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42064</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>42065</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>42066</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>42067</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>42068</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>42069</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>42070</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42071</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>42072</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>42073</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>42074</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>42075</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="14">
                   <c:v>42076</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="15">
+                  <c:v>42077</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42078</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>42079</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="18">
                   <c:v>42080</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="19">
                   <c:v>42081</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="20">
                   <c:v>42082</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="21">
                   <c:v>42083</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22">
+                  <c:v>42084</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>42085</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>42086</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="25">
                   <c:v>42087</c:v>
                 </c:pt>
               </c:numCache>
@@ -362,24 +434,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$19</c:f>
+              <c:f>Sheet1!$C$2:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>126</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>124</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>112.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>112.5</c:v>
@@ -397,16 +469,16 @@
                   <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>107.5</c:v>
+                  <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>107.5</c:v>
+                  <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>107.5</c:v>
+                  <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>107.5</c:v>
+                  <c:v>112.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>107.5</c:v>
@@ -418,6 +490,30 @@
                   <c:v>107.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>107.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>107.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>107.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>107.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>107.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>107.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>107.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>107.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>107.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -849,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,8 +973,8 @@
         <v>42062</v>
       </c>
       <c r="B2" s="1">
-        <f t="shared" ref="B2:B17" si="0">B3+10.8</f>
-        <v>183.60000000000005</v>
+        <f t="shared" ref="B2:B25" si="0">B3+10.8</f>
+        <v>270.00000000000011</v>
       </c>
       <c r="C2" s="1">
         <v>128</v>
@@ -886,102 +982,102 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
+        <v>42063</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" si="0"/>
+        <v>259.2000000000001</v>
+      </c>
+      <c r="C3" s="1">
+        <f>C2</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>42064</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" si="0"/>
+        <v>248.40000000000012</v>
+      </c>
+      <c r="C4" s="1">
+        <f>C3</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>42065</v>
       </c>
-      <c r="B3" s="1">
-        <f t="shared" si="0"/>
-        <v>172.80000000000004</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>237.60000000000011</v>
+      </c>
+      <c r="C5" s="1">
         <f>C2-2</f>
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>42066</v>
-      </c>
-      <c r="B4" s="1">
-        <f t="shared" si="0"/>
-        <v>162.00000000000003</v>
-      </c>
-      <c r="C4" s="1">
-        <f>C3-2</f>
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>42067</v>
-      </c>
-      <c r="B5" s="1">
-        <f t="shared" si="0"/>
-        <v>151.20000000000002</v>
-      </c>
-      <c r="C5" s="1">
-        <f>C4-124+112.5</f>
-        <v>112.5</v>
-      </c>
-    </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>42068</v>
+        <v>42066</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
-        <v>140.4</v>
+        <v>226.8000000000001</v>
       </c>
       <c r="C6" s="1">
-        <f>C5</f>
-        <v>112.5</v>
+        <f>C5-2</f>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>42069</v>
+        <v>42067</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
-        <v>129.6</v>
+        <v>216.00000000000009</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" ref="C7:C19" si="1">C6</f>
+        <f>C6-124+112.5</f>
         <v>112.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>42072</v>
+        <v>42068</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v>118.79999999999998</v>
+        <v>205.20000000000007</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="1"/>
+        <f>C7</f>
         <v>112.5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>42073</v>
+        <v>42069</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
-        <v>107.99999999999999</v>
+        <v>194.40000000000006</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C9:C11" si="1">C8</f>
         <v>112.5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>42074</v>
+        <v>42070</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>97.199999999999989</v>
+        <v>183.60000000000005</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="1"/>
@@ -990,11 +1086,11 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>42075</v>
+        <v>42071</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>86.399999999999991</v>
+        <v>172.80000000000004</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="1"/>
@@ -1003,105 +1099,209 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>42076</v>
+        <v>42072</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>75.599999999999994</v>
+        <v>162.00000000000003</v>
       </c>
       <c r="C12" s="1">
-        <f>C11-5</f>
-        <v>107.5</v>
+        <f>C9</f>
+        <v>112.5</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>42079</v>
+        <v>42073</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
-        <v>64.8</v>
+        <v>151.20000000000002</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
+        <f>C12</f>
+        <v>112.5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>42080</v>
+        <v>42074</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>140.4</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
+        <f>C13</f>
+        <v>112.5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>42081</v>
+        <v>42075</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
-        <v>43.2</v>
+        <v>129.6</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" si="1"/>
-        <v>107.5</v>
+        <f>C14</f>
+        <v>112.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>42082</v>
+        <v>42076</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
-        <v>32.400000000000006</v>
+        <v>118.79999999999998</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" si="1"/>
+        <f>C15-5</f>
         <v>107.5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>42083</v>
+        <v>42077</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
-        <v>21.6</v>
+        <v>107.99999999999999</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" si="1"/>
+        <f>C16</f>
         <v>107.5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>42086</v>
+        <v>42078</v>
       </c>
       <c r="B18" s="1">
-        <f>B19+10.8</f>
-        <v>10.8</v>
+        <f t="shared" si="0"/>
+        <v>97.199999999999989</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" si="1"/>
+        <f>C17</f>
         <v>107.5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
+        <v>42079</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="0"/>
+        <v>86.399999999999991</v>
+      </c>
+      <c r="C19" s="1">
+        <f>C16</f>
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>42080</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>75.599999999999994</v>
+      </c>
+      <c r="C20" s="1">
+        <f>C19</f>
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>42081</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="0"/>
+        <v>64.8</v>
+      </c>
+      <c r="C21" s="1">
+        <f>C20</f>
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>42082</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="C22" s="1">
+        <f>C21</f>
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>42083</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" si="0"/>
+        <v>43.2</v>
+      </c>
+      <c r="C23" s="1">
+        <f>C22</f>
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>42084</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="0"/>
+        <v>32.400000000000006</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" ref="C24:C25" si="2">C23</f>
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>42085</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="0"/>
+        <v>21.6</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="2"/>
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>42086</v>
+      </c>
+      <c r="B26" s="1">
+        <f>B27+10.8</f>
+        <v>10.8</v>
+      </c>
+      <c r="C26" s="1">
+        <f>C23</f>
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>42087</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B27" s="1">
         <v>0</v>
       </c>
-      <c r="C19" s="1">
-        <f t="shared" si="1"/>
+      <c r="C27" s="1">
+        <f>C26</f>
         <v>107.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started EL Conversion and Recommendations
</commit_message>
<xml_diff>
--- a/Burn Down Chart.xlsx
+++ b/Burn Down Chart.xlsx
@@ -15,7 +15,6 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -157,7 +156,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -742,11 +740,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="152783872"/>
-        <c:axId val="152790144"/>
+        <c:axId val="163011584"/>
+        <c:axId val="163030528"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="152783872"/>
+        <c:axId val="163011584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -768,21 +766,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="mmmm\ d" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152790144"/>
+        <c:crossAx val="163030528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="152790144"/>
+        <c:axId val="163030528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -805,21 +802,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152783872"/>
+        <c:crossAx val="163011584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -971,55 +966,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>75</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>65</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1137,28 +1132,28 @@
                   <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>63</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>63</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>63</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>63</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>63</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>63</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>63</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>63</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1175,11 +1170,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="165332480"/>
-        <c:axId val="165334016"/>
+        <c:axId val="167551360"/>
+        <c:axId val="171227776"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="165332480"/>
+        <c:axId val="167551360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1208,14 +1203,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165334016"/>
+        <c:crossAx val="171227776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="165334016"/>
+        <c:axId val="171227776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1245,7 +1240,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165332480"/>
+        <c:crossAx val="167551360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2187,10 +2182,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2216,8 +2211,8 @@
         <v>42102</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B16" si="0">B3+5</f>
-        <v>80</v>
+        <f t="shared" ref="B2:B19" si="0">B3+5</f>
+        <v>95</v>
       </c>
       <c r="C2" s="1">
         <v>63</v>
@@ -2229,7 +2224,7 @@
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1">
         <f>C2</f>
@@ -2242,10 +2237,10 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:C18" si="1">C3</f>
+        <f t="shared" ref="C4:C21" si="1">C3</f>
         <v>63</v>
       </c>
     </row>
@@ -2255,7 +2250,7 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="1"/>
@@ -2268,7 +2263,7 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="1"/>
@@ -2281,7 +2276,7 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="1"/>
@@ -2294,7 +2289,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="1"/>
@@ -2307,7 +2302,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="1"/>
@@ -2320,7 +2315,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="1"/>
@@ -2333,11 +2328,11 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" si="1"/>
-        <v>63</v>
+        <f>C10-6</f>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2346,11 +2341,11 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2359,11 +2354,11 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2372,11 +2367,11 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2385,11 +2380,11 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2398,11 +2393,11 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2410,12 +2405,12 @@
         <v>42117</v>
       </c>
       <c r="B17">
-        <f>B18+5</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2423,15 +2418,51 @@
         <v>42118</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>42119</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="1"/>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
+      <c r="A20" s="2">
+        <v>42120</v>
+      </c>
+      <c r="B20">
+        <f>B21+5</f>
+        <v>5</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>42121</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UI Fixes for US15
</commit_message>
<xml_diff>
--- a/Burn Down Chart.xlsx
+++ b/Burn Down Chart.xlsx
@@ -1190,7 +1190,7 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2222,7 +2222,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2497,8 +2497,8 @@
         <v>0</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" si="1"/>
-        <v>36</v>
+        <f>C20-19</f>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Don't Cry Out Loud
</commit_message>
<xml_diff>
--- a/Burn Down Chart.xlsx
+++ b/Burn Down Chart.xlsx
@@ -157,6 +157,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -767,6 +768,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="mmmm\ d" sourceLinked="1"/>
@@ -803,6 +805,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -816,6 +819,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1190,7 +1194,7 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1658,7 +1662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C42"/>
     </sheetView>
   </sheetViews>
@@ -2497,8 +2501,8 @@
         <v>0</v>
       </c>
       <c r="C21" s="1">
-        <f>C20-29</f>
-        <v>7</v>
+        <f>C20-36</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>